<commit_message>
Adding STM32 - not quite complete addition to lbr
don't use it!
</commit_message>
<xml_diff>
--- a/rage datasheets/bom.xlsx
+++ b/rage datasheets/bom.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rebeccali\Documents\GitHub\kiwitroller\rage datasheets\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="42195" windowHeight="20505"/>
+    <workbookView xWindow="1755" yWindow="30" windowWidth="42195" windowHeight="20505"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>HP1-1400LD</t>
   </si>
@@ -46,19 +51,75 @@
   </si>
   <si>
     <t>IXDD609</t>
+  </si>
+  <si>
+    <t>Part</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Qty</t>
+  </si>
+  <si>
+    <t>Unit Price</t>
+  </si>
+  <si>
+    <t>SUPER TOTAL:</t>
+  </si>
+  <si>
+    <t>Schematic Name (if applicable)</t>
+  </si>
+  <si>
+    <t>Digikey link</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>rated to input voltage, shottcky</t>
+  </si>
+  <si>
+    <t>B170-FDICT-ND</t>
+  </si>
+  <si>
+    <t>Diode LM5007</t>
+  </si>
+  <si>
+    <t>rectifier</t>
+  </si>
+  <si>
+    <t>48-15v reg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -69,7 +130,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -77,12 +138,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF999999"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF999999"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -92,6 +178,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -140,7 +229,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -175,7 +264,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -384,173 +473,403 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1">
+    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
         <v>2.09</v>
-      </c>
-      <c r="C1">
-        <v>1</v>
-      </c>
-      <c r="D1">
-        <f>B1*C1</f>
-        <v>2.09</v>
-      </c>
-      <c r="F1">
-        <f>SUM(D1:D10)</f>
-        <v>14.463270000000001</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>0.95062000000000002</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:D10" si="0">B2*C2</f>
+        <f>B2*C2</f>
+        <v>2.09</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="1">
+        <f>SUM(D2:D11)</f>
+        <v>14.463270000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
         <v>0.95062000000000002</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>0.3135</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D3:D40" si="0">B3*C3</f>
+        <v>0.95062000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
         <v>0.3135</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>0.16320000000000001</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
+        <v>0.3135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
         <v>0.16320000000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>1.4624999999999999</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
+        <v>0.16320000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
         <v>1.4624999999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>1.4624999999999999</v>
+      </c>
+      <c r="G6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <v>0.14105000000000001</v>
       </c>
-      <c r="C6">
+      <c r="C7">
         <v>5</v>
       </c>
-      <c r="D6">
+      <c r="D7">
         <f t="shared" si="0"/>
         <v>0.70525000000000004</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="G7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="B8">
         <v>0.21</v>
       </c>
-      <c r="C7">
+      <c r="C8">
         <v>1</v>
       </c>
-      <c r="D7">
+      <c r="D8">
         <f t="shared" si="0"/>
         <v>0.21</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="B9">
         <v>0.51870000000000005</v>
       </c>
-      <c r="C8">
+      <c r="C9">
         <v>6</v>
       </c>
-      <c r="D8">
+      <c r="D9">
         <f t="shared" si="0"/>
         <v>3.1122000000000005</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="B10">
         <v>0.04</v>
       </c>
-      <c r="C9">
+      <c r="C10">
         <v>23</v>
       </c>
-      <c r="D9">
+      <c r="D10">
         <f t="shared" si="0"/>
         <v>0.92</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B10">
+      <c r="B11">
         <v>0.75600000000000001</v>
       </c>
-      <c r="C10">
+      <c r="C11">
         <v>6</v>
       </c>
-      <c r="D10">
+      <c r="D11">
         <f t="shared" si="0"/>
         <v>4.5359999999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15">
+        <v>0.21</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>0.21</v>
+      </c>
+      <c r="E15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D36">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D39">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D40">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>